<commit_message>
Final changes, but errors
</commit_message>
<xml_diff>
--- a/PW statistics.xlsx
+++ b/PW statistics.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\own\github\Parallel-Dev-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\parallel dev (XPGMCH)\Parallel-Dev-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC2817-593A-45EF-A0B1-A92B2D8865D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56241A6-0CF7-4BFF-9C28-E0AA337529D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Without parallel code:</t>
   </si>
@@ -54,112 +65,7 @@
     <t>Group size:</t>
   </si>
   <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>5.86</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>1.038</t>
-  </si>
-  <si>
-    <t>0.142</t>
-  </si>
-  <si>
-    <t>5.913</t>
-  </si>
-  <si>
-    <t>0.286</t>
-  </si>
-  <si>
-    <t>5.71</t>
-  </si>
-  <si>
-    <t>0.00058</t>
-  </si>
-  <si>
-    <t>1.272</t>
-  </si>
-  <si>
-    <t>0.087</t>
-  </si>
-  <si>
-    <t>7.842</t>
-  </si>
-  <si>
-    <t>1070.928</t>
-  </si>
-  <si>
-    <t>2610.193</t>
-  </si>
-  <si>
-    <t>0.191</t>
-  </si>
-  <si>
-    <t>4.654</t>
-  </si>
-  <si>
-    <t>1831.657</t>
-  </si>
-  <si>
-    <t>3141.782</t>
-  </si>
-  <si>
-    <t>0.2221</t>
-  </si>
-  <si>
-    <t>6.1200</t>
-  </si>
-  <si>
-    <t>20451.674</t>
-  </si>
-  <si>
-    <t>32.2300</t>
-  </si>
-  <si>
-    <t>33.94</t>
-  </si>
-  <si>
-    <t>26312.458</t>
-  </si>
-  <si>
-    <t>28870.271</t>
-  </si>
-  <si>
-    <t>30412.4</t>
-  </si>
-  <si>
-    <t>0.112</t>
-  </si>
-  <si>
-    <t>0.122</t>
-  </si>
-  <si>
-    <t>0.192</t>
-  </si>
-  <si>
-    <t>0.21</t>
-  </si>
-  <si>
-    <t>3.762</t>
-  </si>
-  <si>
-    <t>4.012</t>
-  </si>
-  <si>
-    <t>21.67</t>
-  </si>
-  <si>
-    <t>30.452</t>
-  </si>
-  <si>
-    <t>45.645</t>
-  </si>
-  <si>
-    <t>42.023</t>
+    <t>Speed up</t>
   </si>
 </sst>
 </file>
@@ -201,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -210,6 +116,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -490,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,9 +411,10 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -518,7 +426,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -537,8 +445,11 @@
       <c r="I2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -548,8 +459,8 @@
       <c r="C3">
         <v>15000</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="D3">
+        <v>0.3</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -560,19 +471,23 @@
       <c r="H3">
         <v>15000</v>
       </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>5.86</v>
+      </c>
+      <c r="K3" s="4">
+        <f>I3/D3</f>
+        <v>19.533333333333335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>10000</v>
       </c>
       <c r="C4">
         <v>32000</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="D4">
+        <v>0.28599999999999998</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -583,19 +498,23 @@
       <c r="H4">
         <v>32000</v>
       </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>5.71</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" ref="K4:K22" si="0">I4/D4</f>
+        <v>19.965034965034967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1000000</v>
       </c>
       <c r="C5">
         <v>15000</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
+      <c r="D5">
+        <v>1070.9280000000001</v>
       </c>
       <c r="F5">
         <v>1000</v>
@@ -606,19 +525,23 @@
       <c r="H5">
         <v>15000</v>
       </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2610.1930000000002</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="0"/>
+        <v>2.4373188486994457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1000000</v>
       </c>
       <c r="C6">
         <v>32000</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
+      <c r="D6">
+        <v>1831.6569999999999</v>
       </c>
       <c r="G6" s="1">
         <v>1000000</v>
@@ -626,19 +549,23 @@
       <c r="H6">
         <v>32000</v>
       </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>3141.7820000000002</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7152676510940641</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>100000000</v>
       </c>
       <c r="C7">
         <v>15000</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
+      <c r="D7">
+        <v>20451.673999999999</v>
       </c>
       <c r="G7" s="1">
         <v>100000000</v>
@@ -646,19 +573,23 @@
       <c r="H7">
         <v>15000</v>
       </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>28870.271000000001</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4116336393783708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>100000000</v>
       </c>
       <c r="C8">
         <v>32000</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
+      <c r="D8">
+        <v>26312.457999999999</v>
       </c>
       <c r="G8" s="1">
         <v>100000000</v>
@@ -666,11 +597,15 @@
       <c r="H8">
         <v>32000</v>
       </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>30412.400000000001</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1558175218749993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -680,8 +615,8 @@
       <c r="C10">
         <v>15000</v>
       </c>
-      <c r="D10" t="s">
-        <v>17</v>
+      <c r="D10">
+        <v>5.8E-4</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -692,19 +627,23 @@
       <c r="H10">
         <v>15000</v>
       </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1.038</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="0"/>
+        <v>1789.6551724137933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10000</v>
       </c>
       <c r="C11">
         <v>32000</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
+      <c r="D11">
+        <v>1E-3</v>
       </c>
       <c r="G11">
         <v>10000</v>
@@ -712,19 +651,23 @@
       <c r="H11">
         <v>32000</v>
       </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1.272</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="0"/>
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>1000000</v>
       </c>
       <c r="C12">
         <v>15000</v>
       </c>
-      <c r="D12" t="s">
-        <v>23</v>
+      <c r="D12">
+        <v>0.191</v>
       </c>
       <c r="G12" s="1">
         <v>1000000</v>
@@ -732,19 +675,23 @@
       <c r="H12">
         <v>15000</v>
       </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>4.6539999999999999</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="0"/>
+        <v>24.366492146596858</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>1000000</v>
       </c>
       <c r="C13">
         <v>32000</v>
       </c>
-      <c r="D13" t="s">
-        <v>27</v>
+      <c r="D13">
+        <v>0.22209999999999999</v>
       </c>
       <c r="G13" s="1">
         <v>1000000</v>
@@ -752,19 +699,23 @@
       <c r="H13">
         <v>32000</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>6.12</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="0"/>
+        <v>27.555155335434492</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>100000000</v>
       </c>
       <c r="C14">
         <v>15000</v>
       </c>
-      <c r="D14" t="s">
-        <v>39</v>
+      <c r="D14">
+        <v>3.762</v>
       </c>
       <c r="G14" s="1">
         <v>100000000</v>
@@ -772,19 +723,23 @@
       <c r="H14">
         <v>15000</v>
       </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>21.67</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="0"/>
+        <v>5.7602339181286553</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>100000000</v>
       </c>
       <c r="C15">
         <v>32000</v>
       </c>
-      <c r="D15" t="s">
-        <v>40</v>
+      <c r="D15">
+        <v>4.0119999999999996</v>
       </c>
       <c r="G15" s="1">
         <v>100000000</v>
@@ -792,11 +747,15 @@
       <c r="H15">
         <v>32000</v>
       </c>
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>30.452000000000002</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="0"/>
+        <v>7.5902293120638102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -806,8 +765,8 @@
       <c r="C17">
         <v>15000</v>
       </c>
-      <c r="D17" t="s">
-        <v>13</v>
+      <c r="D17">
+        <v>0.14199999999999999</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -818,19 +777,23 @@
       <c r="H17">
         <v>15000</v>
       </c>
-      <c r="I17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>5.9130000000000003</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="0"/>
+        <v>41.640845070422543</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>10000</v>
       </c>
       <c r="C18">
         <v>32000</v>
       </c>
-      <c r="D18" t="s">
-        <v>19</v>
+      <c r="D18">
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="G18">
         <v>10000</v>
@@ -838,19 +801,23 @@
       <c r="H18">
         <v>32000</v>
       </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>7.8419999999999996</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="0"/>
+        <v>90.137931034482762</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>1000000</v>
       </c>
       <c r="C19">
         <v>15000</v>
       </c>
-      <c r="D19" t="s">
-        <v>35</v>
+      <c r="D19">
+        <v>0.112</v>
       </c>
       <c r="G19" s="1">
         <v>1000000</v>
@@ -858,19 +825,23 @@
       <c r="H19">
         <v>15000</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="4">
+        <v>32.229999999999997</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="0"/>
+        <v>287.76785714285711</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>1000000</v>
       </c>
       <c r="C20">
         <v>32000</v>
       </c>
-      <c r="D20" t="s">
-        <v>36</v>
+      <c r="D20">
+        <v>0.122</v>
       </c>
       <c r="G20" s="1">
         <v>1000000</v>
@@ -878,19 +849,23 @@
       <c r="H20">
         <v>32000</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="4">
+        <v>33.94</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="0"/>
+        <v>278.19672131147541</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>100000000</v>
       </c>
       <c r="C21">
         <v>15000</v>
       </c>
-      <c r="D21" t="s">
-        <v>37</v>
+      <c r="D21">
+        <v>0.192</v>
       </c>
       <c r="G21" s="1">
         <v>100000000</v>
@@ -898,19 +873,23 @@
       <c r="H21">
         <v>15000</v>
       </c>
-      <c r="I21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>45.645000000000003</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="0"/>
+        <v>237.734375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>100000000</v>
       </c>
       <c r="C22">
         <v>32000</v>
       </c>
-      <c r="D22" t="s">
-        <v>38</v>
+      <c r="D22">
+        <v>0.21</v>
       </c>
       <c r="G22" s="1">
         <v>100000000</v>
@@ -918,8 +897,12 @@
       <c r="H22">
         <v>32000</v>
       </c>
-      <c r="I22" t="s">
-        <v>44</v>
+      <c r="I22">
+        <v>42.023000000000003</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="0"/>
+        <v>200.10952380952384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>